<commit_message>
test cases and functions mapped with TC number. 2 Invalid cases added
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData.xlsx
+++ b/src/main/resources/TestData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{B0F4F5F4-FEDE-44E1-89A1-DAD3E606DE32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{390ED05D-CD41-408F-A03A-87BF494144E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="39">
   <si>
     <t>admin</t>
   </si>
@@ -127,6 +127,18 @@
   </si>
   <si>
     <t>Job seeking</t>
+  </si>
+  <si>
+    <t>PR30001</t>
+  </si>
+  <si>
+    <t>Kanakambary</t>
+  </si>
+  <si>
+    <t>TC_41</t>
+  </si>
+  <si>
+    <t>TC_38</t>
   </si>
 </sst>
 </file>
@@ -530,10 +542,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BDE0319-A1DE-487B-A6A9-C7667C55A685}">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -655,6 +667,49 @@
       </c>
       <c r="C6" t="s">
         <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D7" t="s">
+        <v>27</v>
+      </c>
+      <c r="F7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8">
+        <v>123456</v>
+      </c>
+      <c r="D8" t="s">
+        <v>27</v>
+      </c>
+      <c r="E8" t="s">
+        <v>31</v>
+      </c>
+      <c r="F8" t="s">
+        <v>28</v>
+      </c>
+      <c r="G8" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modified Admin and Learners form for update and Delete button
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData.xlsx
+++ b/src/main/resources/TestData.xlsx
@@ -1,18 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{CC20C7A0-0FAA-4AAB-9119-BCA5E4441089}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{135BE697-2D9C-4CF6-8580-D20B8019C520}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3492" yWindow="960" windowWidth="15192" windowHeight="9912" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:O14"/>
+  <oleSize ref="A1:J7"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -490,7 +490,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
@@ -565,7 +565,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BDE0319-A1DE-487B-A6A9-C7667C55A685}">
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>

</xml_diff>